<commit_message>
Updated reactor core recipe chain to be more balanced. Reduced start and stop defaults on reator to match new burn rate.
</commit_message>
<xml_diff>
--- a/Info/recipes_work.xlsx
+++ b/Info/recipes_work.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\All_Programming_Projects\Satisfactory\Satisfactory_PostUpdate3\RP-2.0\SF_Mod_RefinedPower\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514026EC-E2CF-4A87-AB47-F9B89AF65610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E727677-E571-4588-896A-1253ADE91B95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A4D7ED0B-2C8E-4654-AAB9-5A2BAC8D9475}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
   <si>
     <t>Input</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>5000 (5m^3)</t>
-  </si>
-  <si>
-    <t>10 Quartz Crystal + 1 Heavy Modular Frame</t>
   </si>
   <si>
     <t>1000 Unfil Dueterium + 2000 water (2 packed water)</t>
@@ -245,6 +242,12 @@
       </rPr>
       <t xml:space="preserve"> entire settup when considering overflow</t>
     </r>
+  </si>
+  <si>
+    <t>24 Quartz Crystal + 1 Heavy Modular Frame</t>
+  </si>
+  <si>
+    <t>20(10 to stop)</t>
   </si>
 </sst>
 </file>
@@ -779,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02AAF9C9-922D-462E-9CBB-AF887DF673A6}">
   <dimension ref="B1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -820,10 +823,10 @@
         <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -831,7 +834,7 @@
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -860,7 +863,7 @@
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>8</v>
@@ -898,7 +901,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="13">
         <v>1000</v>
@@ -908,7 +911,7 @@
         <v>7500</v>
       </c>
       <c r="H6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.35">
@@ -921,7 +924,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
@@ -940,10 +943,10 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.35">
@@ -960,7 +963,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>8</v>
@@ -978,11 +981,11 @@
         <f>(60/D10)*F10</f>
         <v>0.5</v>
       </c>
-      <c r="I10">
-        <v>375</v>
+      <c r="I10" t="s">
+        <v>63</v>
       </c>
       <c r="J10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K10">
         <f>J13/5000</f>
@@ -1026,7 +1029,7 @@
         <v>100</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.35">
@@ -1062,7 +1065,7 @@
         <v>5000</v>
       </c>
       <c r="H14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.35">
@@ -1115,29 +1118,29 @@
     <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="24"/>
       <c r="C19" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="E19" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="24"/>
       <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="25" t="s">
@@ -1145,12 +1148,12 @@
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2">
         <f>(2000*60)/D2</f>
@@ -1167,12 +1170,12 @@
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2">
         <f>C21</f>
@@ -1185,12 +1188,12 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1200,7 +1203,7 @@
         <v>7500</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.35">
@@ -1214,36 +1217,36 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="24"/>
       <c r="C25" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="E25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="F25" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="24"/>
       <c r="C26" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="2">
         <f>(2000*60)/D4</f>
@@ -1262,7 +1265,7 @@
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="2">
         <f>F23</f>
@@ -1277,7 +1280,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1299,34 +1302,34 @@
     <row r="31" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B31" s="24"/>
       <c r="C31" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="E31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="F31" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B32" s="24"/>
       <c r="C32" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B33" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="2">
         <f>(1000*60)/D6</f>
@@ -1344,7 +1347,7 @@
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2">
         <f>F29</f>
@@ -1358,7 +1361,7 @@
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B35" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1379,34 +1382,34 @@
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" s="24"/>
       <c r="C37" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="24" t="s">
+      <c r="E37" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="F37" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" s="24"/>
       <c r="C38" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39" s="2">
         <f>(10*60)/D8</f>
@@ -1424,7 +1427,7 @@
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B40" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" s="2">
         <f>C39</f>
@@ -1439,7 +1442,7 @@
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B41" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -1449,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
@@ -1463,25 +1466,25 @@
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B43" s="24"/>
       <c r="C43" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="E43" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E43" s="12" t="s">
+      <c r="F43" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="F43" s="12" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" s="24"/>
       <c r="C44" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="27" t="s">
@@ -1490,7 +1493,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45" s="2">
         <f>(1*60)/D10</f>
@@ -1508,7 +1511,7 @@
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" s="2">
         <f>F41</f>
@@ -1523,7 +1526,7 @@
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B47" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -1533,7 +1536,7 @@
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.35">

</xml_diff>